<commit_message>
add portfolioüberblick for M4
</commit_message>
<xml_diff>
--- a/documentation/Portfolioüberblick-Anteile.xlsx
+++ b/documentation/Portfolioüberblick-Anteile.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t>Dokument</t>
   </si>
@@ -163,6 +163,60 @@
   </si>
   <si>
     <t>1.10 GUI-Mockups</t>
+  </si>
+  <si>
+    <t>Aktivitätsdiagramm.vsd</t>
+  </si>
+  <si>
+    <t>Aktivtätsdiagramm</t>
+  </si>
+  <si>
+    <t>Klassendiagram.vsd</t>
+  </si>
+  <si>
+    <t>Klassendiagramm</t>
+  </si>
+  <si>
+    <t>Komponentendiagramm.vsd</t>
+  </si>
+  <si>
+    <t>Komponentendiagramm</t>
+  </si>
+  <si>
+    <t>seq_dia_reservation_v2.vsd</t>
+  </si>
+  <si>
+    <t>Sequenzdiagramm</t>
+  </si>
+  <si>
+    <t>Zustandsdiagramm.vsd</t>
+  </si>
+  <si>
+    <t>Zustandsdiagramm</t>
+  </si>
+  <si>
+    <t>FST17_M4_Aerzteapp.doc</t>
+  </si>
+  <si>
+    <t>1 Architekturkonzept</t>
+  </si>
+  <si>
+    <t>2 Komponentendiagramm</t>
+  </si>
+  <si>
+    <t>4 Sequenzdiagramm</t>
+  </si>
+  <si>
+    <t>5 Aktivitätsdiagramm</t>
+  </si>
+  <si>
+    <t>6 Zustandsdiagramm</t>
+  </si>
+  <si>
+    <t>7 Realisierungstechnologien</t>
+  </si>
+  <si>
+    <t>3 Grobentwurf (Klassendiagramm)</t>
   </si>
 </sst>
 </file>
@@ -489,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:XFD30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,7 +659,7 @@
         <v>100</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I29" si="0">SUM(E4:H4)</f>
+        <f t="shared" ref="I4:I41" si="0">SUM(E4:H4)</f>
         <v>100</v>
       </c>
     </row>
@@ -1274,6 +1328,330 @@
         <v>10</v>
       </c>
       <c r="I29">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>4</v>
+      </c>
+      <c r="B30" t="s">
+        <v>45</v>
+      </c>
+      <c r="D30" t="s">
+        <v>46</v>
+      </c>
+      <c r="E30">
+        <v>10</v>
+      </c>
+      <c r="F30">
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>10</v>
+      </c>
+      <c r="H30">
+        <v>70</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31">
+        <v>10</v>
+      </c>
+      <c r="F31">
+        <v>70</v>
+      </c>
+      <c r="G31">
+        <v>10</v>
+      </c>
+      <c r="H31">
+        <v>10</v>
+      </c>
+      <c r="I31">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <v>30</v>
+      </c>
+      <c r="G32">
+        <v>30</v>
+      </c>
+      <c r="H32">
+        <v>10</v>
+      </c>
+      <c r="I32">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+      <c r="E33">
+        <v>10</v>
+      </c>
+      <c r="F33">
+        <v>10</v>
+      </c>
+      <c r="G33">
+        <v>70</v>
+      </c>
+      <c r="H33">
+        <v>10</v>
+      </c>
+      <c r="I33">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
+      </c>
+      <c r="F34">
+        <v>30</v>
+      </c>
+      <c r="G34">
+        <v>30</v>
+      </c>
+      <c r="H34">
+        <v>10</v>
+      </c>
+      <c r="I34">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35">
+        <v>70</v>
+      </c>
+      <c r="F35">
+        <v>10</v>
+      </c>
+      <c r="G35">
+        <v>10</v>
+      </c>
+      <c r="H35">
+        <v>10</v>
+      </c>
+      <c r="I35">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>4</v>
+      </c>
+      <c r="B36" t="s">
+        <v>55</v>
+      </c>
+      <c r="C36" t="s">
+        <v>57</v>
+      </c>
+      <c r="E36">
+        <v>10</v>
+      </c>
+      <c r="F36">
+        <v>70</v>
+      </c>
+      <c r="G36">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>10</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>4</v>
+      </c>
+      <c r="B37" t="s">
+        <v>55</v>
+      </c>
+      <c r="C37" t="s">
+        <v>62</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>70</v>
+      </c>
+      <c r="G37">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <v>10</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>55</v>
+      </c>
+      <c r="C38" t="s">
+        <v>58</v>
+      </c>
+      <c r="E38">
+        <v>10</v>
+      </c>
+      <c r="F38">
+        <v>10</v>
+      </c>
+      <c r="G38">
+        <v>70</v>
+      </c>
+      <c r="H38">
+        <v>10</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>4</v>
+      </c>
+      <c r="B39" t="s">
+        <v>55</v>
+      </c>
+      <c r="C39" t="s">
+        <v>59</v>
+      </c>
+      <c r="E39">
+        <v>10</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>10</v>
+      </c>
+      <c r="H39">
+        <v>70</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40">
+        <v>70</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+      <c r="G40">
+        <v>10</v>
+      </c>
+      <c r="H40">
+        <v>10</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>4</v>
+      </c>
+      <c r="B41" t="s">
+        <v>55</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E41">
+        <v>70</v>
+      </c>
+      <c r="F41">
+        <v>10</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+      <c r="H41">
+        <v>10</v>
+      </c>
+      <c r="I41">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>

</xml_diff>